<commit_message>
4- and 3-values dividers added
</commit_message>
<xml_diff>
--- a/doc/Keypad-divider-values.xlsx
+++ b/doc/Keypad-divider-values.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="7-values" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="4-values" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="3-values" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t xml:space="preserve">R, ohm</t>
   </si>
@@ -89,6 +91,30 @@
   </si>
   <si>
     <t xml:space="preserve">Total:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3K3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2K2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K</t>
   </si>
 </sst>
 </file>
@@ -211,19 +237,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.75"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.09183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -400,13 +429,482 @@
         <v>15221.6216216216</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2200</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <f aca="false">C12*D13/(1024-D13)</f>
+        <v>365.831435079727</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>360</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <f aca="false">((C12*D14)+C13*(D14-1024))/(1024-D14)</f>
+        <v>511.764193335574</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">D13+$D$3</f>
+        <v>292</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>510</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <f aca="false">((D15*C12)+C13*(D15-1024)+C14*(D15-1024))/(1024-D15)</f>
+        <v>766.772972267293</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">D14+$D$3</f>
+        <v>438</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>750</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">SUM(C12:C15)</f>
+        <v>3844.36860068259</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.92857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.03061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.27040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.60204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.92857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <f aca="false">C2*D3/(1024-D3)</f>
+        <v>1100</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">H4/2</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <f aca="false">((C2*D4)+C3*(D4-1024))/(1024-D4)</f>
+        <v>2200</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">D3+$D$3</f>
+        <v>512</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">1024/4</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">((D5*C2)+C3*(D5-1024)+C4*(D5-1024))/(1024-D5)</f>
+        <v>6600</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">D4+$D$3</f>
+        <v>768</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">(H4+H6)/2</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <f aca="false">SUM(C2:C5)</f>
+        <v>13200</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="H6" s="0" t="n">
+        <f aca="false">H4*2</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="0" t="n">
+        <f aca="false">(H6+H8)/2</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <f aca="false">H4*3</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="0" t="n">
+        <f aca="false">(H8+H10)/2</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <v>1024</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.16326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.65816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.18877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.02040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.39285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.33673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.09183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>6800</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <f aca="false">C2*D3/(1024-D3)</f>
+        <v>3395.02196193265</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <f aca="false">I4/2</f>
+        <v>170.666666666667</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <f aca="false">((C2*D4)+C3*(D4-1024))/(1024-D4)</f>
+        <v>10224.919387041</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>683</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <f aca="false">I8/3</f>
+        <v>341.333333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>20419.9413489736</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="J5" s="6" t="n">
+        <f aca="false">(I6+I4)/2</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1"/>
+      <c r="I6" s="6" t="n">
+        <f aca="false">I4*2</f>
+        <v>682.666666666667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1"/>
+      <c r="J7" s="6" t="n">
+        <f aca="false">(I6+I8)/2</f>
+        <v>853.333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="1"/>
+      <c r="I8" s="0" t="n">
+        <v>1024</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for 2-values divider
</commit_message>
<xml_diff>
--- a/doc/Keypad-divider-values.xlsx
+++ b/doc/Keypad-divider-values.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="7-values" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="4-values" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="3-values" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2-values" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t xml:space="preserve">R, ohm</t>
   </si>
@@ -245,14 +246,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.85714285714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.75"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.09183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="38.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -558,19 +559,19 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.92857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.91326530612245"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.26530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.03061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.27040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.60204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.92857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.28571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,22 +752,22 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.16326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.65816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.18877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.02040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.39285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.33673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.09183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.15816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.51020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -823,10 +824,10 @@
       </c>
       <c r="C3" s="6" t="n">
         <f aca="false">C2*D3/(1024-D3)</f>
-        <v>3395.02196193265</v>
+        <v>3380.11695906433</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>25</v>
@@ -848,7 +849,7 @@
       </c>
       <c r="C4" s="6" t="n">
         <f aca="false">((C2*D4)+C3*(D4-1024))/(1024-D4)</f>
-        <v>10224.919387041</v>
+        <v>10239.8243899093</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>683</v>
@@ -860,7 +861,7 @@
         <v>27</v>
       </c>
       <c r="I4" s="6" t="n">
-        <f aca="false">I8/3</f>
+        <f aca="false">1024/3</f>
         <v>341.333333333333</v>
       </c>
     </row>
@@ -895,6 +896,143 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="1"/>
       <c r="I8" s="0" t="n">
+        <v>1024</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.15816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.51020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6632653061225"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>6800</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <f aca="false">C2*D3/(1024-D3)</f>
+        <v>6800</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <f aca="false">I4/2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>13600</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="J5" s="6" t="n">
+        <f aca="false">(I6+I4)/2</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1"/>
+      <c r="I6" s="6" t="n">
         <v>1024</v>
       </c>
     </row>

</xml_diff>